<commit_message>
instructions 6 and data
</commit_message>
<xml_diff>
--- a/new_instructions_6.xlsx
+++ b/new_instructions_6.xlsx
@@ -47,7 +47,7 @@
     <t xml:space="preserve">Please press “1” if you think the sentence is in the same “part” as the sentence before. </t>
   </si>
   <si>
-    <t xml:space="preserve">There are no “right” answers. We want to see what you think these transitions are. </t>
+    <t xml:space="preserve">There are no “right” answers. We want to see what you think these parts are. </t>
   </si>
   <si>
     <t xml:space="preserve">When you make the decision that each sentence is beginning a new part of the story or not by pressing "9" or "1", you will advance to the next sentence. </t>
@@ -69,7 +69,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -77,6 +77,11 @@
     </font>
     <font>
       <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
@@ -92,7 +97,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +119,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -304,37 +315,37 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -359,6 +370,7 @@
       <rgbColor rgb="ffcccccc"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="fff1c232"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
@@ -376,10 +388,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="404040"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="BFBFBF"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="499BC9"/>
@@ -573,14 +585,15 @@
   <a:objectDefaults>
     <a:spDef>
       <a:spPr>
-        <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
-          <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
-        </a:blipFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst>
           <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
@@ -595,35 +608,29 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
-                <a:srgbClr val="000000">
-                  <a:alpha val="31034"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
             <a:uFillTx/>
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
@@ -876,14 +883,20 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="6350" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1172,7 +1185,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1455,9 +1468,7 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>

</xml_diff>